<commit_message>
Add degree req script
</commit_message>
<xml_diff>
--- a/backend/database/degreereqs/DegreeReqs.xlsx
+++ b/backend/database/degreereqs/DegreeReqs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RobbieZhuang/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/RobbieZhuang/sandbox/school/cs348/CS348Project/backend/database/degreereqs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E01F06AE-713D-7046-A32A-CB4D10873B2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67BE2055-AB5E-184E-8762-ED18388C53CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13040" yWindow="2300" windowWidth="20580" windowHeight="17980" xr2:uid="{01BDD313-82F3-3744-BA3D-655E12DDD30F}"/>
+    <workbookView xWindow="6420" yWindow="1560" windowWidth="20580" windowHeight="17980" xr2:uid="{01BDD313-82F3-3744-BA3D-655E12DDD30F}"/>
   </bookViews>
   <sheets>
     <sheet name="Computer Science" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="169">
   <si>
     <t>CS 115</t>
   </si>
@@ -543,9 +543,6 @@
   </si>
   <si>
     <t>PMATH 365</t>
-  </si>
-  <si>
-    <t>(from table 2)</t>
   </si>
 </sst>
 </file>
@@ -937,8 +934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F4070AB-DA91-1340-B0E3-4D6454BE7855}">
   <dimension ref="A1:AF33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q36" sqref="Q36"/>
+    <sheetView tabSelected="1" topLeftCell="O3" workbookViewId="0">
+      <selection activeCell="R28" sqref="R28:AA28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1272,7 +1269,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:27">
+    <row r="17" spans="1:17">
       <c r="A17" t="s">
         <v>99</v>
       </c>
@@ -1292,108 +1289,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:27">
-      <c r="A18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:27">
-      <c r="A19" t="s">
-        <v>133</v>
-      </c>
-      <c r="B19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27">
-      <c r="A20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27">
-      <c r="A21" t="s">
-        <v>134</v>
-      </c>
-      <c r="B21" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:27">
-      <c r="A22" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:27">
-      <c r="A23" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:27">
-      <c r="A24" t="s">
-        <v>135</v>
-      </c>
-      <c r="B24" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="25" spans="1:27">
-      <c r="A25" t="s">
-        <v>105</v>
-      </c>
-      <c r="B25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" t="s">
-        <v>106</v>
-      </c>
-      <c r="D25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:27">
-      <c r="A26" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:27">
-      <c r="A27" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:27">
+    <row r="28" spans="1:17">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1443,36 +1339,6 @@
         <v>1</v>
       </c>
       <c r="Q28">
-        <v>1</v>
-      </c>
-      <c r="R28">
-        <v>1</v>
-      </c>
-      <c r="S28">
-        <v>1</v>
-      </c>
-      <c r="T28">
-        <v>1</v>
-      </c>
-      <c r="U28">
-        <v>1</v>
-      </c>
-      <c r="V28">
-        <v>1</v>
-      </c>
-      <c r="W28">
-        <v>1</v>
-      </c>
-      <c r="X28">
-        <v>1</v>
-      </c>
-      <c r="Y28">
-        <v>1</v>
-      </c>
-      <c r="Z28">
-        <v>1</v>
-      </c>
-      <c r="AA28">
         <v>1</v>
       </c>
     </row>
@@ -1487,10 +1353,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A9A4D74-8770-D445-92BE-E5E8B3154D42}">
-  <dimension ref="A1:T25"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="K32" sqref="H32:K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1669,110 +1535,9 @@
       </c>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
-      <c r="A12" t="s">
-        <v>133</v>
-      </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="A14" t="s">
-        <v>134</v>
-      </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20">
-      <c r="A17" t="s">
-        <v>135</v>
-      </c>
-      <c r="B17" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20">
-      <c r="A18" t="s">
-        <v>105</v>
-      </c>
-      <c r="B18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" t="s">
-        <v>106</v>
-      </c>
-      <c r="D18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20">
+      <c r="E11" s="6"/>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1801,36 +1566,6 @@
         <v>1</v>
       </c>
       <c r="J25">
-        <v>1</v>
-      </c>
-      <c r="K25">
-        <v>1</v>
-      </c>
-      <c r="L25">
-        <v>1</v>
-      </c>
-      <c r="M25">
-        <v>1</v>
-      </c>
-      <c r="N25">
-        <v>1</v>
-      </c>
-      <c r="O25">
-        <v>1</v>
-      </c>
-      <c r="P25">
-        <v>1</v>
-      </c>
-      <c r="Q25">
-        <v>1</v>
-      </c>
-      <c r="R25">
-        <v>1</v>
-      </c>
-      <c r="S25">
-        <v>1</v>
-      </c>
-      <c r="T25">
         <v>1</v>
       </c>
     </row>
@@ -1841,10 +1576,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{920DD181-FD71-1549-8204-8BBA5E616139}">
-  <dimension ref="A1:S21"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="D19" sqref="A10:D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1979,110 +1714,9 @@
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" t="s">
-        <v>133</v>
-      </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" t="s">
-        <v>134</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" t="s">
-        <v>135</v>
-      </c>
-      <c r="B16" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19">
-      <c r="A17" t="s">
-        <v>105</v>
-      </c>
-      <c r="B17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" t="s">
-        <v>106</v>
-      </c>
-      <c r="D17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19">
-      <c r="A19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19">
+      <c r="E10" s="7"/>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21">
         <v>1</v>
       </c>
@@ -2108,36 +1742,6 @@
         <v>1</v>
       </c>
       <c r="I21">
-        <v>1</v>
-      </c>
-      <c r="J21">
-        <v>1</v>
-      </c>
-      <c r="K21">
-        <v>1</v>
-      </c>
-      <c r="L21">
-        <v>1</v>
-      </c>
-      <c r="M21">
-        <v>1</v>
-      </c>
-      <c r="N21">
-        <v>1</v>
-      </c>
-      <c r="O21">
-        <v>1</v>
-      </c>
-      <c r="P21">
-        <v>1</v>
-      </c>
-      <c r="Q21">
-        <v>1</v>
-      </c>
-      <c r="R21">
-        <v>1</v>
-      </c>
-      <c r="S21">
         <v>1</v>
       </c>
     </row>

</xml_diff>